<commit_message>
Update task import template
</commit_message>
<xml_diff>
--- a/docs/Template/Import_Task_Template.xlsx
+++ b/docs/Template/Import_Task_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15440"/>
+    <workbookView windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="数据" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="85">
   <si>
     <r>
       <rPr>
@@ -61,6 +61,9 @@
     </r>
   </si>
   <si>
+    <t>缺陷等级</t>
+  </si>
+  <si>
     <t>测试类型</t>
   </si>
   <si>
@@ -89,6 +92,15 @@
     <t>确认人</t>
   </si>
   <si>
+    <t>测试人</t>
+  </si>
+  <si>
+    <t>是否漏测缺陷</t>
+  </si>
+  <si>
+    <t>是否计划任务</t>
+  </si>
+  <si>
     <t>优先级</t>
   </si>
   <si>
@@ -108,6 +120,9 @@
   </si>
   <si>
     <t>任务状态</t>
+  </si>
+  <si>
+    <t>软件版本</t>
   </si>
   <si>
     <t>开始时间</t>
@@ -246,6 +261,12 @@
     <t>否</t>
   </si>
   <si>
+    <t>致命|严重|一般|轻微</t>
+  </si>
+  <si>
+    <t>严重</t>
+  </si>
+  <si>
     <t>性能测试|功能测试|稳定性测试|自定义测试</t>
   </si>
   <si>
@@ -264,6 +285,18 @@
     <t>刘德强</t>
   </si>
   <si>
+    <t>苏娜</t>
+  </si>
+  <si>
+    <t>是/否</t>
+  </si>
+  <si>
+    <t>缺陷类型任务时，不指定默认为”否“</t>
+  </si>
+  <si>
+    <t>不指定默认为”否“</t>
+  </si>
+  <si>
     <t>最高|高|中|低|最低</t>
   </si>
   <si>
@@ -295,6 +328,12 @@
   </si>
   <si>
     <t>已完成</t>
+  </si>
+  <si>
+    <t>最长40字符</t>
+  </si>
+  <si>
+    <t>V1.0</t>
   </si>
   <si>
     <t>2024-06-02 23:59:59</t>
@@ -1002,7 +1041,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1028,9 +1067,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1588,77 +1624,81 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="29.3269230769231" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.1923076923077" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.9519230769231" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.4615384615385" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.0288461538462" style="10" customWidth="1"/>
-    <col min="6" max="6" width="12.0096153846154" style="10" customWidth="1"/>
-    <col min="7" max="7" width="22.7596153846154" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.4230769230769" style="14" customWidth="1"/>
-    <col min="9" max="9" width="31.5673076923077" style="10" customWidth="1"/>
-    <col min="10" max="10" width="15.7019230769231" style="15" customWidth="1"/>
-    <col min="11" max="11" width="15.5384615384615" style="15" customWidth="1"/>
-    <col min="12" max="12" width="13.7788461538462" style="10" customWidth="1"/>
-    <col min="13" max="13" width="21.1442307692308" style="14" customWidth="1"/>
-    <col min="14" max="14" width="22.9038461538462" style="14" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="14" customWidth="1"/>
-    <col min="16" max="16" width="20.1826923076923" style="14" customWidth="1"/>
-    <col min="17" max="17" width="17.7884615384615" style="14" customWidth="1"/>
-    <col min="18" max="18" width="24.8365384615385" style="14" customWidth="1"/>
-    <col min="19" max="19" width="32.6923076923077" style="10" customWidth="1"/>
-    <col min="20" max="20" width="27.8846153846154" style="16" customWidth="1"/>
-    <col min="21" max="21" width="20.3461538461538" style="16" customWidth="1"/>
-    <col min="22" max="22" width="18.9038461538462" style="14" customWidth="1"/>
-    <col min="23" max="16384" width="9.23076923076923" style="10"/>
+    <col min="1" max="1" width="29.3269230769231" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.1923076923077" style="9" customWidth="1"/>
+    <col min="3" max="4" width="21.9519230769231" style="9" customWidth="1"/>
+    <col min="5" max="5" width="17.4615384615385" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.0288461538462" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.0096153846154" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.7019230769231" style="9" customWidth="1"/>
+    <col min="9" max="9" width="15.5480769230769" style="9" customWidth="1"/>
+    <col min="10" max="10" width="12.0096153846154" style="9" customWidth="1"/>
+    <col min="11" max="11" width="22.7596153846154" style="13" customWidth="1"/>
+    <col min="12" max="12" width="18.4230769230769" style="13" customWidth="1"/>
+    <col min="13" max="13" width="31.5673076923077" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15.7019230769231" style="14" customWidth="1"/>
+    <col min="15" max="15" width="15.5384615384615" style="14" customWidth="1"/>
+    <col min="16" max="16" width="13.7788461538462" style="9" customWidth="1"/>
+    <col min="17" max="17" width="15.375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="21.1442307692308" style="13" customWidth="1"/>
+    <col min="19" max="19" width="22.9038461538462" style="13" customWidth="1"/>
+    <col min="20" max="20" width="20.5" style="13" customWidth="1"/>
+    <col min="21" max="21" width="20.1826923076923" style="13" customWidth="1"/>
+    <col min="22" max="22" width="17.7884615384615" style="13" customWidth="1"/>
+    <col min="23" max="23" width="24.8365384615385" style="13" customWidth="1"/>
+    <col min="24" max="24" width="32.6923076923077" style="9" customWidth="1"/>
+    <col min="25" max="25" width="27.8846153846154" style="15" customWidth="1"/>
+    <col min="26" max="26" width="20.3461538461538" style="15" customWidth="1"/>
+    <col min="27" max="27" width="18.9038461538462" style="13" customWidth="1"/>
+    <col min="28" max="16384" width="9.23076923076923" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" spans="1:22">
-      <c r="A1" s="17" t="s">
+    <row r="1" ht="17" spans="1:27">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="14" t="s">
@@ -1667,25 +1707,40 @@
       <c r="O1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="16"/>
+      <c r="V1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1696,10 +1751,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1721,7 +1776,7 @@
   <sheetData>
     <row r="1" ht="45" customHeight="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
@@ -1732,60 +1787,60 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="13"/>
     </row>
     <row r="3" ht="17" spans="1:6">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="17" spans="1:6">
@@ -1793,19 +1848,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1813,145 +1868,154 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
       <c r="F5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" ht="17" spans="1:7">
-      <c r="A6" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" ht="17" spans="1:7">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:6">
-      <c r="A10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
+      <c r="B10" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1959,220 +2023,205 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:6">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>36</v>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>37</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" customFormat="1" spans="1:7">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2180,22 +2229,22 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2203,22 +2252,137 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" spans="1:7">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix and Optimise task import
</commit_message>
<xml_diff>
--- a/docs/Template/Import_Task_Template.xlsx
+++ b/docs/Template/Import_Task_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15460" activeTab="1"/>
+    <workbookView windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="数据" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="86">
   <si>
     <r>
       <rPr>
@@ -98,7 +98,7 @@
     <t>是否漏测缺陷</t>
   </si>
   <si>
-    <t>是否计划任务</t>
+    <t>是否计划外任务</t>
   </si>
   <si>
     <t>优先级</t>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>缺陷类型任务时，不指定默认为”否“</t>
+  </si>
+  <si>
+    <t>是否计划任务</t>
   </si>
   <si>
     <t>不指定默认为”否“</t>
@@ -1626,8 +1629,8 @@
   <sheetPr/>
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1639,7 +1642,7 @@
     <col min="6" max="6" width="16.0288461538462" style="9" customWidth="1"/>
     <col min="7" max="7" width="12.0096153846154" style="9" customWidth="1"/>
     <col min="8" max="8" width="15.7019230769231" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.5480769230769" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17.9423076923077" style="9" customWidth="1"/>
     <col min="10" max="10" width="12.0096153846154" style="9" customWidth="1"/>
     <col min="11" max="11" width="22.7596153846154" style="13" customWidth="1"/>
     <col min="12" max="12" width="18.4230769230769" style="13" customWidth="1"/>
@@ -1753,7 +1756,7 @@
   <sheetPr/>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -2015,7 +2018,7 @@
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2029,13 +2032,13 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2052,10 +2055,10 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:6">
@@ -2075,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2086,7 +2089,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -2095,7 +2098,7 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2106,13 +2109,13 @@
         <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2">
         <v>2</v>
@@ -2126,13 +2129,13 @@
         <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
@@ -2149,13 +2152,13 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2166,7 +2169,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
@@ -2175,7 +2178,7 @@
         <v>37</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2192,13 +2195,13 @@
         <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2215,13 +2218,13 @@
         <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2238,13 +2241,13 @@
         <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2261,13 +2264,13 @@
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2284,13 +2287,13 @@
         <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2301,7 +2304,7 @@
         <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -2310,10 +2313,10 @@
         <v>37</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:7">
@@ -2324,7 +2327,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
@@ -2333,10 +2336,10 @@
         <v>37</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2359,7 +2362,7 @@
         <v>49</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2376,13 +2379,13 @@
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>